<commit_message>
Update to data and tool with WG-SS
</commit_message>
<xml_diff>
--- a/data-raw/REACH_2024_MSNA-kobo-tool_draft_v10.xlsx
+++ b/data-raw/REACH_2024_MSNA-kobo-tool_draft_v10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/raphael_bacot_impact-initiatives_org/Documents/git/humind/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guillaume.noblet\Documents\GitHub\humind\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="13_ncr:1_{167789E5-FC15-43A5-8409-582F20352593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{188EA2E2-9B3F-49E9-B278-F1C46AFB4903}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B259D4BC-F608-493A-9FAA-F6A519E5131D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D4BD6A84-72CE-494A-A45D-2F376291FCC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D4BD6A84-72CE-494A-A45D-2F376291FCC5}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -6050,12 +6050,6 @@
     <t>Lire les options de réponse à voix haute.</t>
   </si>
   <si>
-    <t>Individual diffiulty seeing</t>
-  </si>
-  <si>
-    <t>Individual diffiulty hearing</t>
-  </si>
-  <si>
     <t>Individual difficulty walking</t>
   </si>
   <si>
@@ -6096,6 +6090,12 @@
   </si>
   <si>
     <t>En utilisant sa langue habituelle, a-t-il/elle des difficultés à communiquer, par exemple à comprendre ou à se faire comprendre ? Diriez-vous que...</t>
+  </si>
+  <si>
+    <t>Individual difficulty seeing</t>
+  </si>
+  <si>
+    <t>Individual difficulty hearing</t>
   </si>
 </sst>
 </file>
@@ -6261,7 +6261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6395,6 +6395,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6403,13 +6407,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6445,10 +6442,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6686,10 +6679,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F2087-EBA3-4A4D-855A-29B5D74B1D94}">
   <dimension ref="A1:Y525"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
@@ -9114,7 +9107,7 @@
       <c r="W54" s="23"/>
       <c r="X54" s="23"/>
     </row>
-    <row r="55" spans="2:24" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:24" ht="13.2" x14ac:dyDescent="0.4">
       <c r="B55" s="9">
         <v>2</v>
       </c>
@@ -9131,10 +9124,10 @@
       <c r="I55" s="14" t="s">
         <v>1887</v>
       </c>
-      <c r="J55" s="51" t="s">
+      <c r="J55" s="14" t="s">
         <v>1915</v>
       </c>
-      <c r="K55" s="51" t="s">
+      <c r="K55" s="14" t="s">
         <v>1916</v>
       </c>
       <c r="L55" s="14"/>
@@ -9204,7 +9197,7 @@
         <v>162</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="11" t="s">
@@ -9228,7 +9221,7 @@
       <c r="P57" s="11"/>
       <c r="Q57" s="11"/>
       <c r="R57" s="11"/>
-      <c r="S57" s="52"/>
+      <c r="S57" s="48"/>
       <c r="T57" s="11"/>
       <c r="U57" s="11"/>
       <c r="V57" s="11"/>
@@ -9249,7 +9242,7 @@
         <v>162</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="11" t="s">
@@ -9274,7 +9267,7 @@
         <v>1921</v>
       </c>
       <c r="Q58" s="11"/>
-      <c r="S58" s="52"/>
+      <c r="S58" s="48"/>
       <c r="T58" s="11"/>
       <c r="U58" s="11"/>
       <c r="V58" s="11"/>
@@ -9295,7 +9288,7 @@
         <v>162</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="11" t="s">
@@ -9320,7 +9313,7 @@
         <v>1922</v>
       </c>
       <c r="Q59" s="11"/>
-      <c r="S59" s="52"/>
+      <c r="S59" s="48"/>
       <c r="T59" s="11"/>
       <c r="U59" s="11"/>
       <c r="V59" s="11"/>
@@ -9341,7 +9334,7 @@
         <v>162</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="11" t="s">
@@ -9365,7 +9358,7 @@
       <c r="P60" s="11" t="s">
         <v>1923</v>
       </c>
-      <c r="Q60" s="52" t="s">
+      <c r="Q60" s="48" t="s">
         <v>1924</v>
       </c>
       <c r="T60" s="11"/>
@@ -9429,7 +9422,7 @@
         <v>162</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>1955</v>
+        <v>1969</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="11" t="s">
@@ -9442,7 +9435,7 @@
         <v>1890</v>
       </c>
       <c r="K62" s="11" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="L62" s="11" t="s">
         <v>1891</v>
@@ -9478,7 +9471,7 @@
         <v>162</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>1956</v>
+        <v>1970</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="11" t="s">
@@ -9491,7 +9484,7 @@
         <v>1893</v>
       </c>
       <c r="K63" s="11" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>1891</v>
@@ -9527,7 +9520,7 @@
         <v>162</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="11" t="s">
@@ -9540,7 +9533,7 @@
         <v>1895</v>
       </c>
       <c r="K64" s="11" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>1891</v>
@@ -9576,7 +9569,7 @@
         <v>162</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="11" t="s">
@@ -9589,7 +9582,7 @@
         <v>1897</v>
       </c>
       <c r="K65" s="11" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="L65" s="11" t="s">
         <v>1891</v>
@@ -9625,7 +9618,7 @@
         <v>162</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="11" t="s">
@@ -9638,7 +9631,7 @@
         <v>1899</v>
       </c>
       <c r="K66" s="11" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="L66" s="11" t="s">
         <v>1891</v>
@@ -9674,7 +9667,7 @@
         <v>162</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="11" t="s">
@@ -9687,7 +9680,7 @@
         <v>1901</v>
       </c>
       <c r="K67" s="11" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="L67" s="11" t="s">
         <v>1891</v>
@@ -19521,8 +19514,8 @@
       <c r="L280" s="33"/>
       <c r="M280" s="33"/>
       <c r="N280" s="33"/>
-      <c r="O280" s="47"/>
-      <c r="P280" s="47"/>
+      <c r="O280" s="49"/>
+      <c r="P280" s="49"/>
       <c r="Q280" s="33"/>
       <c r="R280" s="33"/>
       <c r="S280" s="33"/>
@@ -19616,10 +19609,10 @@
         <v>997</v>
       </c>
       <c r="N282" s="35"/>
-      <c r="O282" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="P282" s="49"/>
+      <c r="O282" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="P282" s="51"/>
       <c r="Q282" s="35"/>
       <c r="R282" s="35"/>
       <c r="S282" s="35"/>
@@ -19664,10 +19657,10 @@
       <c r="L283" s="38"/>
       <c r="M283" s="38"/>
       <c r="N283" s="38"/>
-      <c r="O283" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="P283" s="48"/>
+      <c r="O283" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="P283" s="50"/>
       <c r="Q283" s="38"/>
       <c r="R283" s="38"/>
       <c r="S283" s="38"/>
@@ -19758,10 +19751,10 @@
       <c r="L285" s="38"/>
       <c r="M285" s="38"/>
       <c r="N285" s="38"/>
-      <c r="O285" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="P285" s="48"/>
+      <c r="O285" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="P285" s="50"/>
       <c r="Q285" s="38"/>
       <c r="R285" s="38"/>
       <c r="S285" s="38"/>
@@ -19806,10 +19799,10 @@
       <c r="L286" s="35"/>
       <c r="M286" s="35"/>
       <c r="N286" s="35"/>
-      <c r="O286" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="P286" s="49"/>
+      <c r="O286" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="P286" s="51"/>
       <c r="Q286" s="35"/>
       <c r="R286" s="35"/>
       <c r="S286" s="35"/>
@@ -19854,10 +19847,10 @@
       <c r="L287" s="38"/>
       <c r="M287" s="38"/>
       <c r="N287" s="38"/>
-      <c r="O287" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="P287" s="48"/>
+      <c r="O287" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="P287" s="50"/>
       <c r="Q287" s="38"/>
       <c r="R287" s="38"/>
       <c r="S287" s="38"/>
@@ -19896,8 +19889,8 @@
       <c r="L288" s="33"/>
       <c r="M288" s="33"/>
       <c r="N288" s="33"/>
-      <c r="O288" s="47"/>
-      <c r="P288" s="47"/>
+      <c r="O288" s="49"/>
+      <c r="P288" s="49"/>
       <c r="Q288" s="33"/>
       <c r="R288" s="33"/>
       <c r="S288" s="33"/>
@@ -27213,86 +27206,86 @@
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A459" s="50" t="s">
+      <c r="A459" s="47" t="s">
         <v>1913</v>
       </c>
-      <c r="B459" s="50" t="s">
+      <c r="B459" s="47" t="s">
         <v>1902</v>
       </c>
-      <c r="C459" s="50" t="s">
+      <c r="C459" s="47" t="s">
         <v>1903</v>
       </c>
-      <c r="D459" s="50" t="s">
+      <c r="D459" s="47" t="s">
         <v>1936</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A460" s="50" t="s">
+      <c r="A460" s="47" t="s">
         <v>1913</v>
       </c>
-      <c r="B460" s="50" t="s">
+      <c r="B460" s="47" t="s">
         <v>1904</v>
       </c>
-      <c r="C460" s="50" t="s">
+      <c r="C460" s="47" t="s">
         <v>1905</v>
       </c>
-      <c r="D460" s="50" t="s">
+      <c r="D460" s="47" t="s">
         <v>1937</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A461" s="50" t="s">
+      <c r="A461" s="47" t="s">
         <v>1913</v>
       </c>
-      <c r="B461" s="50" t="s">
+      <c r="B461" s="47" t="s">
         <v>1906</v>
       </c>
-      <c r="C461" s="50" t="s">
+      <c r="C461" s="47" t="s">
         <v>1907</v>
       </c>
-      <c r="D461" s="50" t="s">
+      <c r="D461" s="47" t="s">
         <v>1938</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A462" s="50" t="s">
+      <c r="A462" s="47" t="s">
         <v>1913</v>
       </c>
-      <c r="B462" s="50" t="s">
+      <c r="B462" s="47" t="s">
         <v>1908</v>
       </c>
-      <c r="C462" s="50" t="s">
+      <c r="C462" s="47" t="s">
         <v>1909</v>
       </c>
-      <c r="D462" s="50" t="s">
+      <c r="D462" s="47" t="s">
         <v>1939</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A463" s="50" t="s">
+      <c r="A463" s="47" t="s">
         <v>1913</v>
       </c>
-      <c r="B463" s="50" t="s">
+      <c r="B463" s="47" t="s">
         <v>1910</v>
       </c>
-      <c r="C463" s="50" t="s">
+      <c r="C463" s="47" t="s">
         <v>1911</v>
       </c>
-      <c r="D463" s="50" t="s">
+      <c r="D463" s="47" t="s">
         <v>1940</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A464" s="50" t="s">
+      <c r="A464" s="47" t="s">
         <v>1913</v>
       </c>
-      <c r="B464" s="50" t="s">
+      <c r="B464" s="47" t="s">
         <v>1912</v>
       </c>
-      <c r="C464" s="50" t="s">
+      <c r="C464" s="47" t="s">
         <v>1105</v>
       </c>
-      <c r="D464" s="50" t="s">
+      <c r="D464" s="47" t="s">
         <v>1106</v>
       </c>
     </row>
@@ -27373,15 +27366,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="0abf2ae5-e878-4ccc-836e-24fe06428412">
@@ -27390,6 +27374,15 @@
     <TaxCatchAll xmlns="a6c4a5f2-8fa1-4399-adba-98b13265f581" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27588,20 +27581,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{273B2F34-4A00-4749-8A90-ABD69807953A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4676863E-963D-4151-9B18-83A7B5BD8FFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0abf2ae5-e878-4ccc-836e-24fe06428412"/>
     <ds:schemaRef ds:uri="a6c4a5f2-8fa1-4399-adba-98b13265f581"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{273B2F34-4A00-4749-8A90-ABD69807953A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Change response option to be consistent with rest of IB/Kobo
dnk
pnta
cannot_do
</commit_message>
<xml_diff>
--- a/data-raw/REACH_2024_MSNA-kobo-tool_draft_v10.xlsx
+++ b/data-raw/REACH_2024_MSNA-kobo-tool_draft_v10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guillaume.noblet\Documents\GitHub\humind\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B259D4BC-F608-493A-9FAA-F6A519E5131D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D049434-AF3B-45B1-9DFF-BF2C581147CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D4BD6A84-72CE-494A-A45D-2F376291FCC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{D4BD6A84-72CE-494A-A45D-2F376291FCC5}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1967">
   <si>
     <t>Level</t>
   </si>
@@ -5907,19 +5907,7 @@
     <t>A lot of difficulty</t>
   </si>
   <si>
-    <t>cannot_do_at_all</t>
-  </si>
-  <si>
     <t>Cannot do at all</t>
-  </si>
-  <si>
-    <t>refused_to_answer</t>
-  </si>
-  <si>
-    <t>Refused to answer</t>
-  </si>
-  <si>
-    <t>dont_know</t>
   </si>
   <si>
     <t>l_difficulty</t>
@@ -6005,9 +5993,6 @@
     <t>Pas du tout</t>
   </si>
   <si>
-    <t>Refus de répondre</t>
-  </si>
-  <si>
     <t>Oui [entretien direct]</t>
   </si>
   <si>
@@ -6096,6 +6081,9 @@
   </si>
   <si>
     <t>Individual difficulty hearing</t>
+  </si>
+  <si>
+    <t>cannot_do</t>
   </si>
 </sst>
 </file>
@@ -6679,10 +6667,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F2087-EBA3-4A4D-855A-29B5D74B1D94}">
   <dimension ref="A1:Y525"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
@@ -9125,10 +9113,10 @@
         <v>1887</v>
       </c>
       <c r="J55" s="14" t="s">
-        <v>1915</v>
+        <v>1911</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>1916</v>
+        <v>1912</v>
       </c>
       <c r="L55" s="14"/>
       <c r="M55" s="14"/>
@@ -9164,10 +9152,10 @@
         <v>1886</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>1948</v>
+        <v>1943</v>
       </c>
       <c r="K56" s="11" t="s">
-        <v>1949</v>
+        <v>1944</v>
       </c>
       <c r="L56" s="11"/>
       <c r="M56" s="11"/>
@@ -9197,20 +9185,20 @@
         <v>162</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>1959</v>
+        <v>1954</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="11" t="s">
-        <v>1928</v>
+        <v>1924</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>1917</v>
+        <v>1913</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>1930</v>
+        <v>1926</v>
       </c>
       <c r="K57" s="11" t="s">
-        <v>1950</v>
+        <v>1945</v>
       </c>
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
@@ -9242,20 +9230,20 @@
         <v>162</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>1960</v>
+        <v>1955</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="11" t="s">
-        <v>1929</v>
+        <v>1925</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>1918</v>
+        <v>1914</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>1925</v>
+        <v>1921</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>1951</v>
+        <v>1946</v>
       </c>
       <c r="L58" s="11"/>
       <c r="M58" s="11"/>
@@ -9264,7 +9252,7 @@
         <v>1097</v>
       </c>
       <c r="P58" s="11" t="s">
-        <v>1921</v>
+        <v>1917</v>
       </c>
       <c r="Q58" s="11"/>
       <c r="S58" s="48"/>
@@ -9288,20 +9276,20 @@
         <v>162</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>1961</v>
+        <v>1956</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="11" t="s">
         <v>53</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>1919</v>
+        <v>1915</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>1926</v>
+        <v>1922</v>
       </c>
       <c r="K59" s="11" t="s">
-        <v>1952</v>
+        <v>1947</v>
       </c>
       <c r="L59" s="11"/>
       <c r="M59" s="11"/>
@@ -9310,7 +9298,7 @@
         <v>1097</v>
       </c>
       <c r="P59" s="11" t="s">
-        <v>1922</v>
+        <v>1918</v>
       </c>
       <c r="Q59" s="11"/>
       <c r="S59" s="48"/>
@@ -9334,20 +9322,20 @@
         <v>162</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>1962</v>
+        <v>1957</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="11" t="s">
         <v>58</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>1920</v>
+        <v>1916</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>1927</v>
+        <v>1923</v>
       </c>
       <c r="K60" s="11" t="s">
-        <v>1953</v>
+        <v>1948</v>
       </c>
       <c r="L60" s="11"/>
       <c r="M60" s="11"/>
@@ -9356,10 +9344,10 @@
         <v>1097</v>
       </c>
       <c r="P60" s="11" t="s">
-        <v>1923</v>
+        <v>1919</v>
       </c>
       <c r="Q60" s="48" t="s">
-        <v>1924</v>
+        <v>1920</v>
       </c>
       <c r="T60" s="11"/>
       <c r="U60" s="11"/>
@@ -9382,13 +9370,13 @@
         <v>38</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>1944</v>
+        <v>1939</v>
       </c>
       <c r="J61" s="14" t="s">
-        <v>1945</v>
+        <v>1940</v>
       </c>
       <c r="K61" s="14" t="s">
-        <v>1946</v>
+        <v>1941</v>
       </c>
       <c r="L61" s="14"/>
       <c r="M61" s="14"/>
@@ -9403,7 +9391,7 @@
       <c r="T61" s="14"/>
       <c r="U61" s="14"/>
       <c r="V61" s="14" t="s">
-        <v>1947</v>
+        <v>1942</v>
       </c>
       <c r="W61" s="14"/>
       <c r="X61" s="14"/>
@@ -9422,11 +9410,11 @@
         <v>162</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>1969</v>
+        <v>1964</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="11" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="I62" s="11" t="s">
         <v>1889</v>
@@ -9435,13 +9423,13 @@
         <v>1890</v>
       </c>
       <c r="K62" s="11" t="s">
-        <v>1963</v>
+        <v>1958</v>
       </c>
       <c r="L62" s="11" t="s">
         <v>1891</v>
       </c>
       <c r="M62" s="11" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="N62" s="11"/>
       <c r="O62" s="11" t="s">
@@ -9471,11 +9459,11 @@
         <v>162</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>1970</v>
+        <v>1965</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="11" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="I63" s="11" t="s">
         <v>1892</v>
@@ -9484,13 +9472,13 @@
         <v>1893</v>
       </c>
       <c r="K63" s="11" t="s">
-        <v>1964</v>
+        <v>1959</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>1891</v>
       </c>
       <c r="M63" s="11" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="N63" s="11"/>
       <c r="O63" s="11" t="s">
@@ -9520,11 +9508,11 @@
         <v>162</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="11" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="I64" s="11" t="s">
         <v>1894</v>
@@ -9533,13 +9521,13 @@
         <v>1895</v>
       </c>
       <c r="K64" s="11" t="s">
-        <v>1965</v>
+        <v>1960</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>1891</v>
       </c>
       <c r="M64" s="11" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="N64" s="11"/>
       <c r="O64" s="11" t="s">
@@ -9569,11 +9557,11 @@
         <v>162</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>1956</v>
+        <v>1951</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="11" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="I65" s="11" t="s">
         <v>1896</v>
@@ -9582,13 +9570,13 @@
         <v>1897</v>
       </c>
       <c r="K65" s="11" t="s">
-        <v>1966</v>
+        <v>1961</v>
       </c>
       <c r="L65" s="11" t="s">
         <v>1891</v>
       </c>
       <c r="M65" s="11" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="N65" s="11"/>
       <c r="O65" s="11" t="s">
@@ -9618,11 +9606,11 @@
         <v>162</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>1957</v>
+        <v>1952</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="11" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>1898</v>
@@ -9631,13 +9619,13 @@
         <v>1899</v>
       </c>
       <c r="K66" s="11" t="s">
-        <v>1967</v>
+        <v>1962</v>
       </c>
       <c r="L66" s="11" t="s">
         <v>1891</v>
       </c>
       <c r="M66" s="11" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="N66" s="11"/>
       <c r="O66" s="11" t="s">
@@ -9667,11 +9655,11 @@
         <v>162</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>1958</v>
+        <v>1953</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="11" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>1900</v>
@@ -9680,13 +9668,13 @@
         <v>1901</v>
       </c>
       <c r="K67" s="11" t="s">
-        <v>1968</v>
+        <v>1963</v>
       </c>
       <c r="L67" s="11" t="s">
         <v>1891</v>
       </c>
       <c r="M67" s="11" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="N67" s="11"/>
       <c r="O67" s="11" t="s">
@@ -9717,7 +9705,7 @@
         <v>106</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>1944</v>
+        <v>1939</v>
       </c>
       <c r="J68" s="14"/>
       <c r="K68" s="14"/>
@@ -21480,8 +21468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA255992-FDA4-43C6-8D11-151FA1909D95}">
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView topLeftCell="A452" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B461" sqref="B461"/>
+    <sheetView tabSelected="1" topLeftCell="A449" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B468" sqref="B468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -27207,7 +27195,7 @@
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A459" s="47" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
       <c r="B459" s="47" t="s">
         <v>1902</v>
@@ -27216,12 +27204,12 @@
         <v>1903</v>
       </c>
       <c r="D459" s="47" t="s">
-        <v>1936</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A460" s="47" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
       <c r="B460" s="47" t="s">
         <v>1904</v>
@@ -27230,12 +27218,12 @@
         <v>1905</v>
       </c>
       <c r="D460" s="47" t="s">
-        <v>1937</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A461" s="47" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
       <c r="B461" s="47" t="s">
         <v>1906</v>
@@ -27244,43 +27232,43 @@
         <v>1907</v>
       </c>
       <c r="D461" s="47" t="s">
-        <v>1938</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A462" s="47" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
       <c r="B462" s="47" t="s">
+        <v>1966</v>
+      </c>
+      <c r="C462" s="47" t="s">
         <v>1908</v>
       </c>
-      <c r="C462" s="47" t="s">
-        <v>1909</v>
-      </c>
       <c r="D462" s="47" t="s">
-        <v>1939</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A463" s="47" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
       <c r="B463" s="47" t="s">
-        <v>1910</v>
+        <v>1069</v>
       </c>
       <c r="C463" s="47" t="s">
-        <v>1911</v>
+        <v>1070</v>
       </c>
       <c r="D463" s="47" t="s">
-        <v>1940</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A464" s="47" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
       <c r="B464" s="47" t="s">
-        <v>1912</v>
+        <v>1104</v>
       </c>
       <c r="C464" s="47" t="s">
         <v>1105</v>
@@ -27291,35 +27279,35 @@
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A466" s="26" t="s">
-        <v>1931</v>
+        <v>1927</v>
       </c>
       <c r="B466" s="26" t="s">
-        <v>1932</v>
+        <v>1928</v>
       </c>
       <c r="C466" s="26" t="s">
-        <v>1934</v>
+        <v>1930</v>
       </c>
       <c r="D466" s="26" t="s">
-        <v>1941</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A467" s="26" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B467" s="26" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C467" s="26" t="s">
         <v>1931</v>
       </c>
-      <c r="B467" s="26" t="s">
-        <v>1933</v>
-      </c>
-      <c r="C467" s="26" t="s">
-        <v>1935</v>
-      </c>
       <c r="D467" s="26" t="s">
-        <v>1942</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A468" s="26" t="s">
-        <v>1931</v>
+        <v>1927</v>
       </c>
       <c r="B468" s="26" t="s">
         <v>1100</v>
@@ -27333,7 +27321,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A470" s="26" t="s">
-        <v>1943</v>
+        <v>1938</v>
       </c>
       <c r="B470" s="26" t="s">
         <v>1097</v>
@@ -27347,7 +27335,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A471" s="26" t="s">
-        <v>1943</v>
+        <v>1938</v>
       </c>
       <c r="B471" s="26" t="s">
         <v>1100</v>
@@ -27366,26 +27354,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0abf2ae5-e878-4ccc-836e-24fe06428412">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a6c4a5f2-8fa1-4399-adba-98b13265f581" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080E85EC637DE394385C88CEC49596DF4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cbf0b56eb1933deadc0c0cd1cf77f18f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0abf2ae5-e878-4ccc-836e-24fe06428412" xmlns:ns3="a6c4a5f2-8fa1-4399-adba-98b13265f581" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10b7c0e23eaaa218a26b41bf2b5f2f3d" ns2:_="" ns3:_="">
     <xsd:import namespace="0abf2ae5-e878-4ccc-836e-24fe06428412"/>
@@ -27580,26 +27548,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4676863E-963D-4151-9B18-83A7B5BD8FFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0abf2ae5-e878-4ccc-836e-24fe06428412"/>
-    <ds:schemaRef ds:uri="a6c4a5f2-8fa1-4399-adba-98b13265f581"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{273B2F34-4A00-4749-8A90-ABD69807953A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0abf2ae5-e878-4ccc-836e-24fe06428412">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a6c4a5f2-8fa1-4399-adba-98b13265f581" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFF96905-2111-4460-93B2-5DBBCF58EFBB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27616,4 +27585,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{273B2F34-4A00-4749-8A90-ABD69807953A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4676863E-963D-4151-9B18-83A7B5BD8FFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0abf2ae5-e878-4ccc-836e-24fe06428412"/>
+    <ds:schemaRef ds:uri="a6c4a5f2-8fa1-4399-adba-98b13265f581"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>